<commit_message>
commiting directly with latest changes where generic xpaths has been added to Dynamic Rule and INDB Creation
</commit_message>
<xml_diff>
--- a/Online-INDB/1-Submit_Online-INDB/Online_INDB_Excel.xlsx
+++ b/Online-INDB/1-Submit_Online-INDB/Online_INDB_Excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="INDBID" sheetId="1" state="visible" r:id="rId1"/>
@@ -354,7 +354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
@@ -379,6 +379,27 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>onlineFPtjCXIAH2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>onlinecV6KDHIAAK</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>onlineKDsdDnIAuF</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -391,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -412,7 +433,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>onlinessY67G8A/f</t>
+          <t>onlineAS1DynEAFw</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>onlineWOxEynEAGw</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>onlineddiZynEAKQ</t>
         </is>
       </c>
     </row>
@@ -428,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F1:H2"/>
@@ -493,6 +528,23 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>onlineddiZynEAKQ</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>onlineUVKcynEA1Q</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>onlineZQ2aynEAHI</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -507,8 +559,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>

</xml_diff>